<commit_message>
Updating log with new instructions.
Notes to officer updated, record activity every 20 minutes.
</commit_message>
<xml_diff>
--- a/vza-app/media/VZA-Citation-Log_blank.xlsx
+++ b/vza-app/media/VZA-Citation-Log_blank.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Assign Rosters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amenity/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5779BD01-508D-1349-AF95-BC20561873D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="6030"/>
+    <workbookView xWindow="1360" yWindow="460" windowWidth="33320" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -21,10 +22,16 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">TEMPLATE!$A$1:$L$81</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -287,8 +294,38 @@
     </r>
   </si>
   <si>
+    <t>The following activity log is known to be true and accurate.</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>noon</t>
+  </si>
+  <si>
+    <t>End of Shift</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1. Please document and give reason for any 15-minute periods of No Activity  (See example below)
+      <t xml:space="preserve">1. If 20 minutes pass with no activity, record "No Violation Observed" and the reason why. E.g. "No Violation — bad weather" or "No Violation — street closure nearby." 
 2. Please write clearly and with clarity, </t>
     </r>
     <r>
@@ -317,43 +354,13 @@
     </r>
   </si>
   <si>
-    <t>The following activity log is known to be true and accurate.</t>
-  </si>
-  <si>
-    <t>No Violation Observed During 15-Minute Period</t>
-  </si>
-  <si>
-    <t>4A</t>
-  </si>
-  <si>
-    <t>4C</t>
-  </si>
-  <si>
-    <t>4D</t>
-  </si>
-  <si>
-    <t>4E</t>
-  </si>
-  <si>
-    <t>4F</t>
-  </si>
-  <si>
-    <t>4B</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>noon</t>
-  </si>
-  <si>
-    <t>End of Shift</t>
+    <t>No Violation Observed During 20-Minute Period</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1258,6 +1265,135 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="15" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1270,9 +1406,6 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1300,15 +1433,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1318,12 +1442,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1336,110 +1454,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1448,18 +1467,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1741,53 +1748,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="41" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.5" customWidth="1"/>
+    <col min="12" max="12" width="23.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="115" t="s">
+    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="117"/>
-    </row>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="86"/>
+    </row>
+    <row r="2" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
       <c r="G3" s="34" t="s">
         <v>3</v>
       </c>
@@ -1797,11 +1804,11 @@
       <c r="K3" s="35"/>
       <c r="L3" s="44"/>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="37"/>
       <c r="C4" s="38"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="117"/>
       <c r="G4" s="37"/>
       <c r="H4" s="38"/>
       <c r="I4" s="38"/>
@@ -1809,10 +1816,10 @@
       <c r="K4" s="38"/>
       <c r="L4" s="45"/>
     </row>
-    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="21" x14ac:dyDescent="0.2">
       <c r="B6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1828,7 +1835,7 @@
       <c r="K6" s="40"/>
       <c r="L6" s="44"/>
     </row>
-    <row r="7" spans="2:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="41" t="s">
         <v>40</v>
       </c>
@@ -1844,8 +1851,8 @@
       <c r="K7" s="43"/>
       <c r="L7" s="45"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="105" t="s">
         <v>18</v>
       </c>
@@ -1856,36 +1863,36 @@
       <c r="G9" s="106"/>
       <c r="H9" s="106"/>
       <c r="I9" s="107"/>
-      <c r="J9" s="85" t="s">
+      <c r="J9" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="87"/>
-    </row>
-    <row r="10" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="82"/>
+      <c r="L9" s="83"/>
+    </row>
+    <row r="10" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="14">
         <v>1</v>
       </c>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
       <c r="G10" s="52">
         <v>5</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="77"/>
-      <c r="L10" s="78"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="102"/>
+      <c r="J10" s="118" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="119"/>
+      <c r="L10" s="120"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="15">
         <v>2</v>
       </c>
@@ -1898,15 +1905,15 @@
       <c r="G11" s="53">
         <v>6</v>
       </c>
-      <c r="H11" s="93" t="s">
+      <c r="H11" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="81"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I11" s="131"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="123"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="15">
         <v>3</v>
       </c>
@@ -1919,17 +1926,17 @@
       <c r="G12" s="53">
         <v>7</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="96"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="81"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I12" s="133"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="123"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="108" t="s">
         <v>7</v>
@@ -1944,14 +1951,14 @@
         <v>55</v>
       </c>
       <c r="I13" s="104"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="81"/>
-    </row>
-    <row r="14" spans="2:12" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="121"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="123"/>
+    </row>
+    <row r="14" spans="2:12" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="51"/>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" s="110" t="s">
         <v>50</v>
@@ -1961,144 +1968,144 @@
       <c r="G14" s="53">
         <v>9</v>
       </c>
-      <c r="H14" s="127" t="s">
-        <v>61</v>
-      </c>
-      <c r="I14" s="128"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="84"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="99"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="125"/>
+      <c r="L14" s="126"/>
+    </row>
+    <row r="15" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="51"/>
       <c r="C15" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="112" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="54"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="100"/>
-      <c r="J15" s="85" t="s">
+      <c r="H15" s="91"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="86"/>
-      <c r="L15" s="87"/>
-    </row>
-    <row r="16" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="82"/>
+      <c r="L15" s="83"/>
+    </row>
+    <row r="16" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="51"/>
       <c r="C16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
       <c r="G16" s="55"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="100"/>
-      <c r="J16" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="77"/>
-      <c r="L16" s="78"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="118" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="119"/>
+      <c r="L16" s="120"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="51"/>
       <c r="C17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="112" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="54"/>
-      <c r="H17" s="99"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
-    </row>
-    <row r="18" spans="1:12" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="91"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="122"/>
+      <c r="L17" s="123"/>
+    </row>
+    <row r="18" spans="1:12" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="51"/>
       <c r="C18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
       <c r="G18" s="55"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="100"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="81"/>
-    </row>
-    <row r="19" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="H18" s="91"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="122"/>
+      <c r="L18" s="123"/>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="51"/>
       <c r="C19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
       <c r="G19" s="55"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="100"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="90"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="91"/>
+      <c r="I19" s="92"/>
+      <c r="J19" s="127"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="129"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F20" s="56"/>
       <c r="G20" s="57"/>
-      <c r="H20" s="122"/>
-      <c r="I20" s="122"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
       <c r="J20" s="65"/>
       <c r="K20" s="65"/>
       <c r="L20" s="56"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="F21" s="56"/>
       <c r="G21" s="58"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="123"/>
-      <c r="J21" s="123"/>
-      <c r="K21" s="123"/>
-    </row>
-    <row r="22" spans="1:12" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="94"/>
+    </row>
+    <row r="22" spans="1:12" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101" t="s">
+      <c r="C22" s="100"/>
+      <c r="D22" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
       <c r="G22" s="61" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="101" t="s">
+      <c r="I22" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="101"/>
+      <c r="J22" s="100"/>
       <c r="K22" s="62" t="s">
         <v>45</v>
       </c>
@@ -2106,285 +2113,285 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <v>1</v>
       </c>
-      <c r="B23" s="129"/>
-      <c r="C23" s="129"/>
-      <c r="D23" s="102"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
       <c r="G23" s="68"/>
       <c r="H23" s="59"/>
-      <c r="I23" s="102"/>
-      <c r="J23" s="102"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>2</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
       <c r="G24" s="67"/>
       <c r="H24" s="60"/>
-      <c r="I24" s="130"/>
-      <c r="J24" s="131"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="77"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>3</v>
       </c>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
       <c r="G25" s="67"/>
       <c r="H25" s="60"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>4</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
       <c r="G26" s="67"/>
       <c r="H26" s="60"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>5</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="67"/>
       <c r="H27" s="60"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>6</v>
       </c>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
       <c r="G28" s="67"/>
       <c r="H28" s="60"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>7</v>
       </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
       <c r="G29" s="67"/>
       <c r="H29" s="60"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>8</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
       <c r="G30" s="67"/>
       <c r="H30" s="60"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>9</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
       <c r="G31" s="67"/>
       <c r="H31" s="60"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>10</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
       <c r="G32" s="67"/>
       <c r="H32" s="60"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>11</v>
       </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
       <c r="G33" s="67"/>
       <c r="H33" s="60"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>12</v>
       </c>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
       <c r="G34" s="67"/>
       <c r="H34" s="60"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>13</v>
       </c>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
       <c r="G35" s="67"/>
       <c r="H35" s="60"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="75"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>14</v>
       </c>
-      <c r="B36" s="75"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
       <c r="G36" s="67"/>
       <c r="H36" s="60"/>
-      <c r="I36" s="75"/>
-      <c r="J36" s="75"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="71"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>15</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
       <c r="G37" s="67"/>
       <c r="H37" s="60"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="75"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="124" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="125"/>
-      <c r="C38" s="125"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="125"/>
-      <c r="G38" s="125"/>
-      <c r="H38" s="125"/>
-      <c r="I38" s="125"/>
-      <c r="J38" s="125"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="126"/>
-    </row>
-    <row r="39" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="96"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="96"/>
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="96"/>
+      <c r="L38" s="97"/>
+    </row>
+    <row r="39" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="114" t="s">
+      <c r="B39" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="114"/>
-      <c r="D39" s="114" t="s">
+      <c r="C39" s="78"/>
+      <c r="D39" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="114"/>
-      <c r="F39" s="114"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="64" t="s">
         <v>19</v>
       </c>
       <c r="H39" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="138" t="s">
+      <c r="I39" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="138"/>
+      <c r="J39" s="73"/>
       <c r="K39" s="32" t="s">
         <v>45</v>
       </c>
@@ -2392,799 +2399,745 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="17">
         <v>1</v>
       </c>
-      <c r="B40" s="102"/>
-      <c r="C40" s="102"/>
-      <c r="D40" s="102"/>
-      <c r="E40" s="102"/>
-      <c r="F40" s="102"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
       <c r="G40" s="68"/>
       <c r="H40" s="59"/>
-      <c r="I40" s="137"/>
-      <c r="J40" s="137"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
       <c r="K40" s="33"/>
       <c r="L40" s="33"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>2</v>
       </c>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
       <c r="G41" s="67"/>
       <c r="H41" s="60"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>3</v>
       </c>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
       <c r="G42" s="67"/>
       <c r="H42" s="60"/>
-      <c r="I42" s="75"/>
-      <c r="J42" s="75"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
         <v>4</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
       <c r="G43" s="67"/>
       <c r="H43" s="60"/>
-      <c r="I43" s="75"/>
-      <c r="J43" s="75"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="71"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>5</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
       <c r="G44" s="67"/>
       <c r="H44" s="60"/>
-      <c r="I44" s="75"/>
-      <c r="J44" s="75"/>
+      <c r="I44" s="71"/>
+      <c r="J44" s="71"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>6</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
       <c r="G45" s="67"/>
       <c r="H45" s="60"/>
-      <c r="I45" s="137"/>
-      <c r="J45" s="137"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>7</v>
       </c>
-      <c r="B46" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
+      <c r="B46" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
       <c r="G46" s="67"/>
       <c r="H46" s="60"/>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75"/>
+      <c r="I46" s="71"/>
+      <c r="J46" s="71"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>8</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
       <c r="G47" s="67"/>
       <c r="H47" s="60"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="71"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>9</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="75"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="71"/>
       <c r="G48" s="67"/>
       <c r="H48" s="60"/>
-      <c r="I48" s="75"/>
-      <c r="J48" s="75"/>
+      <c r="I48" s="71"/>
+      <c r="J48" s="71"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>10</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="71"/>
       <c r="G49" s="67"/>
       <c r="H49" s="60"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="75"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>11</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="75"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
       <c r="G50" s="67"/>
       <c r="H50" s="60"/>
-      <c r="I50" s="75"/>
-      <c r="J50" s="75"/>
+      <c r="I50" s="71"/>
+      <c r="J50" s="71"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>12</v>
       </c>
-      <c r="B51" s="75"/>
-      <c r="C51" s="75"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
       <c r="G51" s="67"/>
       <c r="H51" s="60"/>
-      <c r="I51" s="75"/>
-      <c r="J51" s="75"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="71"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>13</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="71"/>
       <c r="G52" s="67"/>
       <c r="H52" s="60"/>
-      <c r="I52" s="75"/>
-      <c r="J52" s="75"/>
+      <c r="I52" s="71"/>
+      <c r="J52" s="71"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>14</v>
       </c>
-      <c r="B53" s="75"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
       <c r="G53" s="67"/>
       <c r="H53" s="60"/>
-      <c r="I53" s="75"/>
-      <c r="J53" s="75"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="71"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>15</v>
       </c>
-      <c r="B54" s="75"/>
-      <c r="C54" s="75"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
+      <c r="B54" s="71"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="71"/>
       <c r="G54" s="67"/>
       <c r="H54" s="60"/>
-      <c r="I54" s="75"/>
-      <c r="J54" s="75"/>
+      <c r="I54" s="71"/>
+      <c r="J54" s="71"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>16</v>
       </c>
-      <c r="B55" s="75"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
+      <c r="B55" s="71"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
       <c r="G55" s="67"/>
       <c r="H55" s="60"/>
-      <c r="I55" s="75"/>
-      <c r="J55" s="75"/>
+      <c r="I55" s="71"/>
+      <c r="J55" s="71"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <v>17</v>
       </c>
-      <c r="B56" s="75"/>
-      <c r="C56" s="75"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
       <c r="G56" s="67"/>
       <c r="H56" s="60"/>
-      <c r="I56" s="75"/>
-      <c r="J56" s="75"/>
+      <c r="I56" s="71"/>
+      <c r="J56" s="71"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>18</v>
       </c>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="71"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="71"/>
       <c r="G57" s="67"/>
       <c r="H57" s="60"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
+      <c r="I57" s="71"/>
+      <c r="J57" s="71"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <v>19</v>
       </c>
-      <c r="B58" s="75"/>
-      <c r="C58" s="75"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
+      <c r="F58" s="71"/>
       <c r="G58" s="67"/>
       <c r="H58" s="60"/>
-      <c r="I58" s="75"/>
-      <c r="J58" s="75"/>
+      <c r="I58" s="71"/>
+      <c r="J58" s="71"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <v>20</v>
       </c>
-      <c r="B59" s="75"/>
-      <c r="C59" s="75"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="71"/>
       <c r="G59" s="67"/>
       <c r="H59" s="60"/>
-      <c r="I59" s="75"/>
-      <c r="J59" s="75"/>
+      <c r="I59" s="71"/>
+      <c r="J59" s="71"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <v>21</v>
       </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="71"/>
       <c r="G60" s="67"/>
       <c r="H60" s="60"/>
-      <c r="I60" s="75"/>
-      <c r="J60" s="75"/>
+      <c r="I60" s="71"/>
+      <c r="J60" s="71"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <v>22</v>
       </c>
-      <c r="B61" s="75"/>
-      <c r="C61" s="75"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="75"/>
-      <c r="F61" s="75"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="71"/>
       <c r="G61" s="67"/>
       <c r="H61" s="60"/>
-      <c r="I61" s="75"/>
-      <c r="J61" s="75"/>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
         <v>23</v>
       </c>
-      <c r="B62" s="75"/>
-      <c r="C62" s="75"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
-      <c r="F62" s="75"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="71"/>
+      <c r="F62" s="71"/>
       <c r="G62" s="67"/>
       <c r="H62" s="60"/>
-      <c r="I62" s="75"/>
-      <c r="J62" s="75"/>
+      <c r="I62" s="71"/>
+      <c r="J62" s="71"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
         <v>24</v>
       </c>
-      <c r="B63" s="75"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
+      <c r="B63" s="71"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="71"/>
+      <c r="F63" s="71"/>
       <c r="G63" s="67"/>
       <c r="H63" s="60"/>
-      <c r="I63" s="75"/>
-      <c r="J63" s="75"/>
+      <c r="I63" s="71"/>
+      <c r="J63" s="71"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>25</v>
       </c>
-      <c r="B64" s="75"/>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="71"/>
       <c r="G64" s="67"/>
       <c r="H64" s="60"/>
-      <c r="I64" s="75"/>
-      <c r="J64" s="75"/>
+      <c r="I64" s="71"/>
+      <c r="J64" s="71"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
         <v>26</v>
       </c>
-      <c r="B65" s="75"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
       <c r="G65" s="67"/>
       <c r="H65" s="60"/>
-      <c r="I65" s="75"/>
-      <c r="J65" s="75"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="71"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <v>27</v>
       </c>
-      <c r="B66" s="75"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="71"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="71"/>
       <c r="G66" s="67"/>
       <c r="H66" s="60"/>
-      <c r="I66" s="75"/>
-      <c r="J66" s="75"/>
+      <c r="I66" s="71"/>
+      <c r="J66" s="71"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <v>28</v>
       </c>
-      <c r="B67" s="75"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
+      <c r="B67" s="71"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="71"/>
+      <c r="F67" s="71"/>
       <c r="G67" s="60"/>
       <c r="H67" s="60"/>
-      <c r="I67" s="75"/>
-      <c r="J67" s="75"/>
+      <c r="I67" s="71"/>
+      <c r="J67" s="71"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <v>29</v>
       </c>
-      <c r="B68" s="75"/>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
+      <c r="B68" s="71"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="71"/>
+      <c r="E68" s="71"/>
+      <c r="F68" s="71"/>
       <c r="G68" s="60"/>
       <c r="H68" s="60"/>
-      <c r="I68" s="75"/>
-      <c r="J68" s="75"/>
+      <c r="I68" s="71"/>
+      <c r="J68" s="71"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>30</v>
       </c>
-      <c r="B69" s="75"/>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
+      <c r="B69" s="71"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="71"/>
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
       <c r="G69" s="60"/>
       <c r="H69" s="60"/>
-      <c r="I69" s="75"/>
-      <c r="J69" s="75"/>
+      <c r="I69" s="71"/>
+      <c r="J69" s="71"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>31</v>
       </c>
-      <c r="B70" s="75"/>
-      <c r="C70" s="75"/>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
+      <c r="B70" s="71"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
       <c r="G70" s="60"/>
       <c r="H70" s="60"/>
-      <c r="I70" s="75"/>
-      <c r="J70" s="75"/>
+      <c r="I70" s="71"/>
+      <c r="J70" s="71"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
         <v>32</v>
       </c>
-      <c r="B71" s="75"/>
-      <c r="C71" s="75"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="75"/>
-      <c r="F71" s="75"/>
+      <c r="B71" s="71"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="71"/>
+      <c r="E71" s="71"/>
+      <c r="F71" s="71"/>
       <c r="G71" s="60"/>
       <c r="H71" s="60"/>
-      <c r="I71" s="75"/>
-      <c r="J71" s="75"/>
+      <c r="I71" s="71"/>
+      <c r="J71" s="71"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
         <v>33</v>
       </c>
-      <c r="B72" s="75"/>
-      <c r="C72" s="75"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
+      <c r="F72" s="71"/>
       <c r="G72" s="60"/>
       <c r="H72" s="60"/>
-      <c r="I72" s="75"/>
-      <c r="J72" s="75"/>
+      <c r="I72" s="71"/>
+      <c r="J72" s="71"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
         <v>34</v>
       </c>
-      <c r="B73" s="75"/>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="71"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="71"/>
       <c r="G73" s="60"/>
       <c r="H73" s="60"/>
-      <c r="I73" s="75"/>
-      <c r="J73" s="75"/>
+      <c r="I73" s="71"/>
+      <c r="J73" s="71"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
         <v>35</v>
       </c>
-      <c r="B74" s="75"/>
-      <c r="C74" s="75"/>
-      <c r="D74" s="75"/>
-      <c r="E74" s="75"/>
-      <c r="F74" s="75"/>
+      <c r="B74" s="71"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="71"/>
+      <c r="F74" s="71"/>
       <c r="G74" s="60"/>
       <c r="H74" s="60"/>
-      <c r="I74" s="75"/>
-      <c r="J74" s="75"/>
+      <c r="I74" s="71"/>
+      <c r="J74" s="71"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <v>36</v>
       </c>
-      <c r="B75" s="75"/>
-      <c r="C75" s="75"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
+      <c r="B75" s="71"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="71"/>
+      <c r="E75" s="71"/>
+      <c r="F75" s="71"/>
       <c r="G75" s="60"/>
       <c r="H75" s="60"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="75"/>
+      <c r="I75" s="71"/>
+      <c r="J75" s="71"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <v>37</v>
       </c>
-      <c r="B76" s="75"/>
-      <c r="C76" s="75"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
+      <c r="B76" s="71"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="71"/>
+      <c r="E76" s="71"/>
+      <c r="F76" s="71"/>
       <c r="G76" s="60"/>
       <c r="H76" s="60"/>
-      <c r="I76" s="75"/>
-      <c r="J76" s="75"/>
+      <c r="I76" s="71"/>
+      <c r="J76" s="71"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
         <v>38</v>
       </c>
-      <c r="B77" s="75"/>
-      <c r="C77" s="75"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
+      <c r="B77" s="71"/>
+      <c r="C77" s="71"/>
+      <c r="D77" s="71"/>
+      <c r="E77" s="71"/>
+      <c r="F77" s="71"/>
       <c r="G77" s="60"/>
       <c r="H77" s="60"/>
-      <c r="I77" s="75"/>
-      <c r="J77" s="75"/>
+      <c r="I77" s="71"/>
+      <c r="J77" s="71"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
         <v>39</v>
       </c>
-      <c r="B78" s="75"/>
-      <c r="C78" s="75"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="75"/>
+      <c r="B78" s="71"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
       <c r="G78" s="60"/>
       <c r="H78" s="60"/>
-      <c r="I78" s="75"/>
-      <c r="J78" s="75"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="71"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
         <v>40</v>
       </c>
-      <c r="B79" s="75"/>
-      <c r="C79" s="75"/>
-      <c r="D79" s="75"/>
-      <c r="E79" s="75"/>
-      <c r="F79" s="75"/>
+      <c r="B79" s="71"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="71"/>
+      <c r="E79" s="71"/>
+      <c r="F79" s="71"/>
       <c r="G79" s="60"/>
       <c r="H79" s="60"/>
-      <c r="I79" s="75"/>
-      <c r="J79" s="75"/>
+      <c r="I79" s="71"/>
+      <c r="J79" s="71"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="118" t="s">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="B80" s="119"/>
-      <c r="C80" s="119"/>
-      <c r="D80" s="119"/>
-      <c r="E80" s="119"/>
-      <c r="F80" s="119"/>
-      <c r="G80" s="119"/>
-      <c r="H80" s="119"/>
-      <c r="I80" s="119"/>
-      <c r="J80" s="119"/>
-      <c r="K80" s="119"/>
-      <c r="L80" s="119"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="120"/>
-      <c r="B81" s="121"/>
-      <c r="C81" s="121"/>
-      <c r="D81" s="121"/>
-      <c r="E81" s="121"/>
-      <c r="F81" s="121"/>
-      <c r="G81" s="121"/>
-      <c r="H81" s="121"/>
-      <c r="I81" s="121"/>
-      <c r="J81" s="121"/>
-      <c r="K81" s="121"/>
-      <c r="L81" s="121"/>
+      <c r="B80" s="88"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="88"/>
+      <c r="E80" s="88"/>
+      <c r="F80" s="88"/>
+      <c r="G80" s="88"/>
+      <c r="H80" s="88"/>
+      <c r="I80" s="88"/>
+      <c r="J80" s="88"/>
+      <c r="K80" s="88"/>
+      <c r="L80" s="88"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" s="89"/>
+      <c r="B81" s="90"/>
+      <c r="C81" s="90"/>
+      <c r="D81" s="90"/>
+      <c r="E81" s="90"/>
+      <c r="F81" s="90"/>
+      <c r="G81" s="90"/>
+      <c r="H81" s="90"/>
+      <c r="I81" s="90"/>
+      <c r="J81" s="90"/>
+      <c r="K81" s="90"/>
+      <c r="L81" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="204">
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="I79:J79"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:F76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="J10:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="A80:L81"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:F40"/>
@@ -3209,69 +3162,123 @@
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="A80:L81"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="J10:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:F77"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="landscape" r:id="rId1"/>
@@ -3282,74 +3289,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="47"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="47"/>
+    <col min="2" max="2" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="135" t="s">
+    <row r="1" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="132" t="s">
+      <c r="C1" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132" t="s">
+      <c r="D1" s="136"/>
+      <c r="E1" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132" t="s">
+      <c r="F1" s="136"/>
+      <c r="G1" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132" t="s">
+      <c r="H1" s="136"/>
+      <c r="I1" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132" t="s">
+      <c r="J1" s="136"/>
+      <c r="K1" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132" t="s">
+      <c r="L1" s="136"/>
+      <c r="M1" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132" t="s">
+      <c r="N1" s="136"/>
+      <c r="O1" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132" t="s">
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132" t="s">
+      <c r="R1" s="136"/>
+      <c r="S1" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="132"/>
-      <c r="U1" s="132" t="s">
+      <c r="T1" s="136"/>
+      <c r="U1" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="132"/>
-      <c r="W1" s="133" t="s">
+      <c r="V1" s="136"/>
+      <c r="W1" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="134"/>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136"/>
-      <c r="B2" s="136"/>
+      <c r="X1" s="138"/>
+    </row>
+    <row r="2" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
       <c r="C2" s="13" t="s">
         <v>33</v>
       </c>
@@ -3417,7 +3424,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>49</v>
       </c>
@@ -3453,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
@@ -3486,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
@@ -3519,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>39</v>
       </c>
@@ -3552,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -3585,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -3618,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>38</v>
       </c>
@@ -3651,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>37</v>
       </c>
@@ -3684,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
@@ -3717,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>35</v>
       </c>
@@ -3750,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
         <v>44</v>
       </c>
@@ -3783,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="31" t="s">
         <v>34</v>
       </c>
@@ -3876,18 +3883,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="B1:B2"/>
@@ -3896,6 +3898,11 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="78" orientation="landscape" r:id="rId1"/>
@@ -3906,74 +3913,74 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19:V29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="47"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="47"/>
+    <col min="2" max="2" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="135" t="s">
+    <row r="1" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="132" t="s">
+      <c r="C1" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132" t="s">
+      <c r="D1" s="136"/>
+      <c r="E1" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132" t="s">
+      <c r="F1" s="136"/>
+      <c r="G1" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132" t="s">
+      <c r="H1" s="136"/>
+      <c r="I1" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132" t="s">
+      <c r="J1" s="136"/>
+      <c r="K1" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132" t="s">
+      <c r="L1" s="136"/>
+      <c r="M1" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132" t="s">
+      <c r="N1" s="136"/>
+      <c r="O1" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132" t="s">
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132" t="s">
+      <c r="R1" s="136"/>
+      <c r="S1" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="132"/>
-      <c r="U1" s="132" t="s">
+      <c r="T1" s="136"/>
+      <c r="U1" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="132"/>
-      <c r="W1" s="133" t="s">
+      <c r="V1" s="136"/>
+      <c r="W1" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="134"/>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136"/>
-      <c r="B2" s="136"/>
+      <c r="X1" s="138"/>
+    </row>
+    <row r="2" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135"/>
+      <c r="B2" s="135"/>
       <c r="C2" s="13" t="s">
         <v>33</v>
       </c>
@@ -4041,7 +4048,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="48">
         <v>42768</v>
       </c>
@@ -4083,7 +4090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
@@ -4116,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
@@ -4149,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4188,7 +4195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -4221,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -4254,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>38</v>
       </c>
@@ -4293,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>37</v>
       </c>
@@ -4329,7 +4336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
@@ -4362,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>35</v>
       </c>
@@ -4395,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
         <v>44</v>
       </c>
@@ -4431,7 +4438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="31" t="s">
         <v>34</v>
       </c>
@@ -4524,67 +4531,67 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="135" t="s">
+    <row r="16" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="132"/>
-      <c r="E17" s="132" t="s">
+      <c r="D17" s="136"/>
+      <c r="E17" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="132"/>
-      <c r="G17" s="132" t="s">
+      <c r="F17" s="136"/>
+      <c r="G17" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="132"/>
-      <c r="I17" s="132" t="s">
+      <c r="H17" s="136"/>
+      <c r="I17" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="132"/>
-      <c r="K17" s="132" t="s">
+      <c r="J17" s="136"/>
+      <c r="K17" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="132"/>
-      <c r="M17" s="132" t="s">
+      <c r="L17" s="136"/>
+      <c r="M17" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="N17" s="132"/>
-      <c r="O17" s="132" t="s">
+      <c r="N17" s="136"/>
+      <c r="O17" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="132"/>
-      <c r="Q17" s="132" t="s">
+      <c r="P17" s="136"/>
+      <c r="Q17" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="R17" s="132"/>
-      <c r="S17" s="132" t="s">
+      <c r="R17" s="136"/>
+      <c r="S17" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="T17" s="132"/>
-      <c r="U17" s="132" t="s">
+      <c r="T17" s="136"/>
+      <c r="U17" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="V17" s="132"/>
-      <c r="W17" s="133" t="s">
+      <c r="V17" s="136"/>
+      <c r="W17" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="X17" s="134"/>
-    </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="136"/>
+      <c r="X17" s="138"/>
+    </row>
+    <row r="18" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="135"/>
+      <c r="B18" s="135"/>
       <c r="C18" s="13" t="s">
         <v>33</v>
       </c>
@@ -4652,7 +4659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="48">
         <v>42769</v>
       </c>
@@ -4688,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="12" t="s">
         <v>31</v>
       </c>
@@ -4721,7 +4728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
         <v>6</v>
       </c>
@@ -4754,7 +4761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
         <v>39</v>
       </c>
@@ -4787,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
         <v>8</v>
       </c>
@@ -4820,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
         <v>9</v>
       </c>
@@ -4853,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
         <v>38</v>
       </c>
@@ -4886,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
         <v>37</v>
       </c>
@@ -4919,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>36</v>
       </c>
@@ -4952,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="12" t="s">
         <v>35</v>
       </c>
@@ -4985,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" s="12" t="s">
         <v>44</v>
       </c>
@@ -5018,7 +5025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="31" t="s">
         <v>34</v>
       </c>
@@ -5113,6 +5120,24 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="S17:T17"/>
     <mergeCell ref="U17:V17"/>
@@ -5121,24 +5146,6 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:V1"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="78" orientation="landscape" r:id="rId1"/>
@@ -5149,69 +5156,69 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="135" t="s">
+    <row r="1" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132" t="s">
+      <c r="C1" s="136"/>
+      <c r="D1" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132" t="s">
+      <c r="E1" s="136"/>
+      <c r="F1" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132" t="s">
+      <c r="G1" s="136"/>
+      <c r="H1" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132" t="s">
+      <c r="I1" s="136"/>
+      <c r="J1" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132" t="s">
+      <c r="K1" s="136"/>
+      <c r="L1" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132" t="s">
+      <c r="M1" s="136"/>
+      <c r="N1" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132" t="s">
+      <c r="O1" s="136"/>
+      <c r="P1" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132" t="s">
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="132"/>
-      <c r="T1" s="132" t="s">
+      <c r="S1" s="136"/>
+      <c r="T1" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="132"/>
-      <c r="V1" s="133" t="s">
+      <c r="U1" s="136"/>
+      <c r="V1" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="134"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136"/>
+      <c r="W1" s="138"/>
+    </row>
+    <row r="2" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135"/>
       <c r="B2" s="13" t="s">
         <v>33</v>
       </c>
@@ -5279,7 +5286,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>30</v>
       </c>
@@ -5318,7 +5325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>31</v>
       </c>
@@ -5354,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
@@ -5399,7 +5406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -5447,7 +5454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5500,7 +5507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5536,7 +5543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
@@ -5593,7 +5600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>37</v>
       </c>
@@ -5644,7 +5651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -5677,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
@@ -5710,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>44</v>
       </c>
@@ -5761,7 +5768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>34</v>
       </c>
@@ -5854,13 +5861,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
@@ -5868,11 +5880,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="78" orientation="landscape" r:id="rId1"/>
@@ -5886,69 +5893,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T3" sqref="T3:U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="135" t="s">
+    <row r="1" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132" t="s">
+      <c r="C1" s="136"/>
+      <c r="D1" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132" t="s">
+      <c r="E1" s="136"/>
+      <c r="F1" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132" t="s">
+      <c r="G1" s="136"/>
+      <c r="H1" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132" t="s">
+      <c r="I1" s="136"/>
+      <c r="J1" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132" t="s">
+      <c r="K1" s="136"/>
+      <c r="L1" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132" t="s">
+      <c r="M1" s="136"/>
+      <c r="N1" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132" t="s">
+      <c r="O1" s="136"/>
+      <c r="P1" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132" t="s">
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="132"/>
-      <c r="T1" s="132" t="s">
+      <c r="S1" s="136"/>
+      <c r="T1" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="132"/>
-      <c r="V1" s="133" t="s">
+      <c r="U1" s="136"/>
+      <c r="V1" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="134"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136"/>
+      <c r="W1" s="138"/>
+    </row>
+    <row r="2" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="135"/>
       <c r="B2" s="13" t="s">
         <v>33</v>
       </c>
@@ -6016,7 +6023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>30</v>
       </c>
@@ -6055,7 +6062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>31</v>
       </c>
@@ -6091,7 +6098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
@@ -6136,7 +6143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -6175,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -6226,7 +6233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
@@ -6271,7 +6278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
@@ -6316,7 +6323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>37</v>
       </c>
@@ -6358,7 +6365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -6391,7 +6398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
@@ -6424,7 +6431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>44</v>
       </c>
@@ -6472,7 +6479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>34</v>
       </c>
@@ -6565,7 +6572,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>43</v>
       </c>

</xml_diff>